<commit_message>
Chapter 4 and Appendix B
Har arbejdet på kapitel 4 samt appendix B
</commit_message>
<xml_diff>
--- a/MiSU-Stat.xlsx
+++ b/MiSU-Stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasMellergaard\Dropbox\Master Projekt\MiSU_Master_Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F8FA67-1776-4397-BC12-F563F1D98C32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C839AB2E-2D9B-43BC-8D4C-7566A326D835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,7 +128,7 @@
     <t>Error</t>
   </si>
   <si>
-    <t>PM</t>
+    <t>+/-</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -356,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -370,34 +370,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -405,9 +405,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,16 +419,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -440,8 +437,18 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -760,54 +767,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="M116" sqref="M116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="2" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="18" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="15" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="45" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="34" t="s">
         <v>33</v>
       </c>
       <c r="I2" s="1"/>
@@ -816,7 +823,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
       <c r="B3" s="6">
@@ -834,11 +841,11 @@
       <c r="F3" s="8">
         <v>3</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="29">
         <f>SUM(B3:F3)</f>
         <v>13</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="29">
         <f>((MAXA(B3:F3)-MINA(B3:F3))/2)</f>
         <v>0.5</v>
       </c>
@@ -848,7 +855,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
       <c r="B4" s="9">
@@ -866,11 +873,11 @@
       <c r="F4" s="10">
         <v>3</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="29">
         <f t="shared" ref="G4:G67" si="0">SUM(B4:F4)</f>
         <v>15</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="29">
         <f t="shared" ref="H4:H67" si="1">((MAXA(B4:F4)-MINA(B4:F4))/2)</f>
         <v>1</v>
       </c>
@@ -880,7 +887,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+      <c r="A5" s="18">
         <v>3</v>
       </c>
       <c r="B5" s="9">
@@ -898,11 +905,11 @@
       <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="29">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -912,7 +919,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <v>4</v>
       </c>
       <c r="B6" s="9">
@@ -930,11 +937,11 @@
       <c r="F6" s="10">
         <v>4</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -944,7 +951,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="18">
         <v>5</v>
       </c>
       <c r="B7" s="9">
@@ -962,11 +969,11 @@
       <c r="F7" s="10">
         <v>2</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -976,7 +983,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="18">
         <v>6</v>
       </c>
       <c r="B8" s="9">
@@ -994,11 +1001,11 @@
       <c r="F8" s="10">
         <v>2</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1008,7 +1015,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="9">
@@ -1026,11 +1033,11 @@
       <c r="F9" s="10">
         <v>2</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1040,7 +1047,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="18">
         <v>8</v>
       </c>
       <c r="B10" s="9">
@@ -1058,11 +1065,11 @@
       <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1072,7 +1079,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="18">
         <v>9</v>
       </c>
       <c r="B11" s="9">
@@ -1090,11 +1097,11 @@
       <c r="F11" s="10">
         <v>2</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="29">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1104,7 +1111,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>10</v>
       </c>
       <c r="B12" s="9">
@@ -1122,11 +1129,11 @@
       <c r="F12" s="10">
         <v>3</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="29">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1136,7 +1143,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>11</v>
       </c>
       <c r="B13" s="9">
@@ -1154,11 +1161,11 @@
       <c r="F13" s="10">
         <v>4</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1168,7 +1175,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="18">
         <v>12</v>
       </c>
       <c r="B14" s="9">
@@ -1186,11 +1193,11 @@
       <c r="F14" s="10">
         <v>3</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1200,7 +1207,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>13</v>
       </c>
       <c r="B15" s="9">
@@ -1218,11 +1225,11 @@
       <c r="F15" s="10">
         <v>1</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1232,7 +1239,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>14</v>
       </c>
       <c r="B16" s="9">
@@ -1250,11 +1257,11 @@
       <c r="F16" s="10">
         <v>1</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1263,8 +1270,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
         <v>15</v>
       </c>
       <c r="B17" s="9">
@@ -1282,11 +1289,11 @@
       <c r="F17" s="10">
         <v>2</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="29">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1296,7 +1303,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>16</v>
       </c>
       <c r="B18" s="9">
@@ -1314,11 +1321,11 @@
       <c r="F18" s="10">
         <v>3</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="29">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H18" s="30">
+      <c r="H18" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1328,7 +1335,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>17</v>
       </c>
       <c r="B19" s="9">
@@ -1346,11 +1353,11 @@
       <c r="F19" s="10">
         <v>3</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="29">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H19" s="30">
+      <c r="H19" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -1360,7 +1367,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>18</v>
       </c>
       <c r="B20" s="9">
@@ -1378,11 +1385,11 @@
       <c r="F20" s="10">
         <v>1</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -1392,7 +1399,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="A21" s="18">
         <v>19</v>
       </c>
       <c r="B21" s="9">
@@ -1410,11 +1417,11 @@
       <c r="F21" s="10">
         <v>7</v>
       </c>
-      <c r="G21" s="31">
+      <c r="G21" s="29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="29">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1424,7 +1431,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="18">
         <v>20</v>
       </c>
       <c r="B22" s="9">
@@ -1442,11 +1449,11 @@
       <c r="F22" s="10">
         <v>3</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="29">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1455,8 +1462,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
         <v>21</v>
       </c>
       <c r="B23" s="9">
@@ -1474,11 +1481,11 @@
       <c r="F23" s="10">
         <v>1</v>
       </c>
-      <c r="G23" s="31">
+      <c r="G23" s="29">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1488,7 +1495,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="18">
         <v>22</v>
       </c>
       <c r="B24" s="9">
@@ -1506,11 +1513,11 @@
       <c r="F24" s="10">
         <v>5</v>
       </c>
-      <c r="G24" s="31">
+      <c r="G24" s="29">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1520,7 +1527,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+      <c r="A25" s="18">
         <v>23</v>
       </c>
       <c r="B25" s="9">
@@ -1538,11 +1545,11 @@
       <c r="F25" s="10">
         <v>6</v>
       </c>
-      <c r="G25" s="31">
+      <c r="G25" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1552,7 +1559,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="18">
         <v>24</v>
       </c>
       <c r="B26" s="9">
@@ -1570,11 +1577,11 @@
       <c r="F26" s="10">
         <v>4</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="29">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1584,7 +1591,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="18">
         <v>25</v>
       </c>
       <c r="B27" s="9">
@@ -1602,11 +1609,11 @@
       <c r="F27" s="10">
         <v>7</v>
       </c>
-      <c r="G27" s="31">
+      <c r="G27" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H27" s="30">
+      <c r="H27" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1616,7 +1623,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="18">
         <v>26</v>
       </c>
       <c r="B28" s="9">
@@ -1634,11 +1641,11 @@
       <c r="F28" s="10">
         <v>6</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="29">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1648,7 +1655,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
+      <c r="A29" s="18">
         <v>27</v>
       </c>
       <c r="B29" s="9">
@@ -1666,11 +1673,11 @@
       <c r="F29" s="10">
         <v>5</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="29">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H29" s="30">
+      <c r="H29" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -1680,7 +1687,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="18">
         <v>28</v>
       </c>
       <c r="B30" s="9">
@@ -1698,11 +1705,11 @@
       <c r="F30" s="10">
         <v>6</v>
       </c>
-      <c r="G30" s="31">
+      <c r="G30" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H30" s="30">
+      <c r="H30" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1712,7 +1719,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+      <c r="A31" s="18">
         <v>29</v>
       </c>
       <c r="B31" s="9">
@@ -1730,11 +1737,11 @@
       <c r="F31" s="10">
         <v>5</v>
       </c>
-      <c r="G31" s="31">
+      <c r="G31" s="29">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H31" s="30">
+      <c r="H31" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1744,7 +1751,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="18">
         <v>30</v>
       </c>
       <c r="B32" s="9">
@@ -1762,11 +1769,11 @@
       <c r="F32" s="10">
         <v>6</v>
       </c>
-      <c r="G32" s="31">
+      <c r="G32" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H32" s="30">
+      <c r="H32" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1776,7 +1783,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
+      <c r="A33" s="18">
         <v>31</v>
       </c>
       <c r="B33" s="9">
@@ -1794,11 +1801,11 @@
       <c r="F33" s="10">
         <v>7</v>
       </c>
-      <c r="G33" s="31">
+      <c r="G33" s="29">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="H33" s="30">
+      <c r="H33" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1808,7 +1815,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="18">
         <v>32</v>
       </c>
       <c r="B34" s="9">
@@ -1826,11 +1833,11 @@
       <c r="F34" s="10">
         <v>6</v>
       </c>
-      <c r="G34" s="31">
+      <c r="G34" s="29">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H34" s="30">
+      <c r="H34" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1840,7 +1847,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
+      <c r="A35" s="18">
         <v>33</v>
       </c>
       <c r="B35" s="9">
@@ -1858,11 +1865,11 @@
       <c r="F35" s="10">
         <v>5</v>
       </c>
-      <c r="G35" s="31">
+      <c r="G35" s="29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H35" s="30">
+      <c r="H35" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -1872,7 +1879,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
+      <c r="A36" s="18">
         <v>34</v>
       </c>
       <c r="B36" s="9">
@@ -1890,11 +1897,11 @@
       <c r="F36" s="10">
         <v>7</v>
       </c>
-      <c r="G36" s="31">
+      <c r="G36" s="29">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H36" s="30">
+      <c r="H36" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -1904,7 +1911,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
+      <c r="A37" s="18">
         <v>35</v>
       </c>
       <c r="B37" s="9">
@@ -1922,11 +1929,11 @@
       <c r="F37" s="10">
         <v>7</v>
       </c>
-      <c r="G37" s="31">
+      <c r="G37" s="29">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H37" s="30">
+      <c r="H37" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1935,8 +1942,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
         <v>36</v>
       </c>
       <c r="B38" s="9">
@@ -1954,11 +1961,11 @@
       <c r="F38" s="10">
         <v>7</v>
       </c>
-      <c r="G38" s="31">
+      <c r="G38" s="29">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H38" s="30">
+      <c r="H38" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1968,7 +1975,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
+      <c r="A39" s="18">
         <v>37</v>
       </c>
       <c r="B39" s="9">
@@ -1986,11 +1993,11 @@
       <c r="F39" s="10">
         <v>5</v>
       </c>
-      <c r="G39" s="31">
+      <c r="G39" s="29">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H39" s="30">
+      <c r="H39" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2000,7 +2007,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
+      <c r="A40" s="18">
         <v>38</v>
       </c>
       <c r="B40" s="9">
@@ -2018,11 +2025,11 @@
       <c r="F40" s="10">
         <v>7</v>
       </c>
-      <c r="G40" s="31">
+      <c r="G40" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H40" s="30">
+      <c r="H40" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2032,7 +2039,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="19">
+      <c r="A41" s="18">
         <v>39</v>
       </c>
       <c r="B41" s="9">
@@ -2050,11 +2057,11 @@
       <c r="F41" s="10">
         <v>5</v>
       </c>
-      <c r="G41" s="31">
+      <c r="G41" s="29">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H41" s="30">
+      <c r="H41" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2064,7 +2071,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
+      <c r="A42" s="18">
         <v>40</v>
       </c>
       <c r="B42" s="9">
@@ -2082,11 +2089,11 @@
       <c r="F42" s="10">
         <v>5</v>
       </c>
-      <c r="G42" s="31">
+      <c r="G42" s="29">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H42" s="30">
+      <c r="H42" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2096,7 +2103,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
+      <c r="A43" s="18">
         <v>41</v>
       </c>
       <c r="B43" s="9">
@@ -2114,11 +2121,11 @@
       <c r="F43" s="10">
         <v>7</v>
       </c>
-      <c r="G43" s="31">
+      <c r="G43" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H43" s="30">
+      <c r="H43" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2128,7 +2135,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="19">
+      <c r="A44" s="18">
         <v>42</v>
       </c>
       <c r="B44" s="9">
@@ -2146,11 +2153,11 @@
       <c r="F44" s="10">
         <v>6</v>
       </c>
-      <c r="G44" s="31">
+      <c r="G44" s="29">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H44" s="30">
+      <c r="H44" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2160,7 +2167,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="19">
+      <c r="A45" s="18">
         <v>43</v>
       </c>
       <c r="B45" s="9">
@@ -2178,11 +2185,11 @@
       <c r="F45" s="10">
         <v>6</v>
       </c>
-      <c r="G45" s="31">
+      <c r="G45" s="29">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H45" s="30">
+      <c r="H45" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2192,7 +2199,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
+      <c r="A46" s="18">
         <v>44</v>
       </c>
       <c r="B46" s="9">
@@ -2210,11 +2217,11 @@
       <c r="F46" s="10">
         <v>7</v>
       </c>
-      <c r="G46" s="31">
+      <c r="G46" s="29">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="H46" s="30">
+      <c r="H46" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2224,7 +2231,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="19">
+      <c r="A47" s="18">
         <v>45</v>
       </c>
       <c r="B47" s="9">
@@ -2242,11 +2249,11 @@
       <c r="F47" s="10">
         <v>5</v>
       </c>
-      <c r="G47" s="31">
+      <c r="G47" s="29">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H47" s="30">
+      <c r="H47" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2256,7 +2263,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
+      <c r="A48" s="18">
         <v>46</v>
       </c>
       <c r="B48" s="9">
@@ -2274,11 +2281,11 @@
       <c r="F48" s="10">
         <v>7</v>
       </c>
-      <c r="G48" s="31">
+      <c r="G48" s="30">
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="H48" s="31">
+      <c r="H48" s="30">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2288,7 +2295,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="19">
+      <c r="A49" s="18">
         <v>47</v>
       </c>
       <c r="B49" s="9">
@@ -2306,11 +2313,11 @@
       <c r="F49" s="10">
         <v>4</v>
       </c>
-      <c r="G49" s="31">
+      <c r="G49" s="29">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H49" s="30">
+      <c r="H49" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2320,7 +2327,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="19">
+      <c r="A50" s="18">
         <v>48</v>
       </c>
       <c r="B50" s="9">
@@ -2338,11 +2345,11 @@
       <c r="F50" s="10">
         <v>6</v>
       </c>
-      <c r="G50" s="31">
+      <c r="G50" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H50" s="30">
+      <c r="H50" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2352,7 +2359,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
+      <c r="A51" s="18">
         <v>49</v>
       </c>
       <c r="B51" s="9">
@@ -2370,11 +2377,11 @@
       <c r="F51" s="10">
         <v>7</v>
       </c>
-      <c r="G51" s="31">
+      <c r="G51" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H51" s="30">
+      <c r="H51" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2384,7 +2391,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="19">
+      <c r="A52" s="18">
         <v>50</v>
       </c>
       <c r="B52" s="9">
@@ -2402,11 +2409,11 @@
       <c r="F52" s="10">
         <v>6</v>
       </c>
-      <c r="G52" s="31">
+      <c r="G52" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H52" s="30">
+      <c r="H52" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2416,7 +2423,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="19">
+      <c r="A53" s="18">
         <v>51</v>
       </c>
       <c r="B53" s="9">
@@ -2434,11 +2441,11 @@
       <c r="F53" s="10">
         <v>5</v>
       </c>
-      <c r="G53" s="31">
+      <c r="G53" s="29">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H53" s="30">
+      <c r="H53" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2448,7 +2455,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="19">
+      <c r="A54" s="18">
         <v>52</v>
       </c>
       <c r="B54" s="9">
@@ -2466,11 +2473,11 @@
       <c r="F54" s="10">
         <v>6</v>
       </c>
-      <c r="G54" s="31">
+      <c r="G54" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H54" s="30">
+      <c r="H54" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2480,7 +2487,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="19">
+      <c r="A55" s="18">
         <v>53</v>
       </c>
       <c r="B55" s="9">
@@ -2498,11 +2505,11 @@
       <c r="F55" s="10">
         <v>6</v>
       </c>
-      <c r="G55" s="31">
+      <c r="G55" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H55" s="30">
+      <c r="H55" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2512,7 +2519,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="19">
+      <c r="A56" s="18">
         <v>54</v>
       </c>
       <c r="B56" s="9">
@@ -2530,11 +2537,11 @@
       <c r="F56" s="10">
         <v>6</v>
       </c>
-      <c r="G56" s="31">
+      <c r="G56" s="29">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="H56" s="30">
+      <c r="H56" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2544,7 +2551,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="19">
+      <c r="A57" s="18">
         <v>55</v>
       </c>
       <c r="B57" s="9">
@@ -2562,11 +2569,11 @@
       <c r="F57" s="10">
         <v>5</v>
       </c>
-      <c r="G57" s="31">
+      <c r="G57" s="29">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H57" s="30">
+      <c r="H57" s="29">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
@@ -2576,7 +2583,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="19">
+      <c r="A58" s="18">
         <v>56</v>
       </c>
       <c r="B58" s="9">
@@ -2594,11 +2601,11 @@
       <c r="F58" s="10">
         <v>6</v>
       </c>
-      <c r="G58" s="31">
+      <c r="G58" s="29">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H58" s="30">
+      <c r="H58" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2608,7 +2615,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="19">
+      <c r="A59" s="18">
         <v>57</v>
       </c>
       <c r="B59" s="9">
@@ -2626,11 +2633,11 @@
       <c r="F59" s="10">
         <v>5</v>
       </c>
-      <c r="G59" s="31">
+      <c r="G59" s="29">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H59" s="30">
+      <c r="H59" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2640,7 +2647,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="19">
+      <c r="A60" s="18">
         <v>58</v>
       </c>
       <c r="B60" s="9">
@@ -2658,11 +2665,11 @@
       <c r="F60" s="10">
         <v>4</v>
       </c>
-      <c r="G60" s="31">
+      <c r="G60" s="29">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H60" s="30">
+      <c r="H60" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2672,7 +2679,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="19">
+      <c r="A61" s="18">
         <v>59</v>
       </c>
       <c r="B61" s="9">
@@ -2690,11 +2697,11 @@
       <c r="F61" s="10">
         <v>4</v>
       </c>
-      <c r="G61" s="31">
+      <c r="G61" s="29">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H61" s="30">
+      <c r="H61" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2704,7 +2711,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="19">
+      <c r="A62" s="18">
         <v>60</v>
       </c>
       <c r="B62" s="9">
@@ -2722,11 +2729,11 @@
       <c r="F62" s="10">
         <v>2</v>
       </c>
-      <c r="G62" s="31">
+      <c r="G62" s="29">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H62" s="30">
+      <c r="H62" s="29">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
@@ -2736,7 +2743,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="19">
+      <c r="A63" s="18">
         <v>61</v>
       </c>
       <c r="B63" s="9">
@@ -2754,11 +2761,11 @@
       <c r="F63" s="10">
         <v>6</v>
       </c>
-      <c r="G63" s="31">
+      <c r="G63" s="29">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H63" s="30">
+      <c r="H63" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2768,7 +2775,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="19">
+      <c r="A64" s="18">
         <v>62</v>
       </c>
       <c r="B64" s="9">
@@ -2786,11 +2793,11 @@
       <c r="F64" s="10">
         <v>4</v>
       </c>
-      <c r="G64" s="31">
+      <c r="G64" s="29">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H64" s="30">
+      <c r="H64" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2800,7 +2807,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="19">
+      <c r="A65" s="18">
         <v>63</v>
       </c>
       <c r="B65" s="9">
@@ -2818,11 +2825,11 @@
       <c r="F65" s="10">
         <v>5</v>
       </c>
-      <c r="G65" s="31">
+      <c r="G65" s="29">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H65" s="30">
+      <c r="H65" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -2832,7 +2839,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="19">
+      <c r="A66" s="18">
         <v>64</v>
       </c>
       <c r="B66" s="9">
@@ -2850,11 +2857,11 @@
       <c r="F66" s="10">
         <v>5</v>
       </c>
-      <c r="G66" s="31">
+      <c r="G66" s="29">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H66" s="30">
+      <c r="H66" s="29">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2864,7 +2871,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="19">
+      <c r="A67" s="18">
         <v>65</v>
       </c>
       <c r="B67" s="9">
@@ -2882,11 +2889,11 @@
       <c r="F67" s="10">
         <v>4</v>
       </c>
-      <c r="G67" s="31">
+      <c r="G67" s="29">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H67" s="30">
+      <c r="H67" s="29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -2896,7 +2903,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="19">
+      <c r="A68" s="18">
         <v>66</v>
       </c>
       <c r="B68" s="9">
@@ -2914,12 +2921,12 @@
       <c r="F68" s="10">
         <v>6</v>
       </c>
-      <c r="G68" s="31">
+      <c r="G68" s="29">
         <f t="shared" ref="G68:G119" si="2">SUM(B68:F68)</f>
         <v>25</v>
       </c>
-      <c r="H68" s="30">
-        <f t="shared" ref="H68:H126" si="3">((MAXA(B68:F68)-MINA(B68:F68))/2)</f>
+      <c r="H68" s="29">
+        <f t="shared" ref="H68:H119" si="3">((MAXA(B68:F68)-MINA(B68:F68))/2)</f>
         <v>1</v>
       </c>
       <c r="I68" s="3"/>
@@ -2928,7 +2935,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="19">
+      <c r="A69" s="18">
         <v>67</v>
       </c>
       <c r="B69" s="9">
@@ -2946,11 +2953,11 @@
       <c r="F69" s="10">
         <v>4</v>
       </c>
-      <c r="G69" s="31">
+      <c r="G69" s="29">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="H69" s="30">
+      <c r="H69" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -2960,7 +2967,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="19">
+      <c r="A70" s="18">
         <v>68</v>
       </c>
       <c r="B70" s="9">
@@ -2978,11 +2985,11 @@
       <c r="F70" s="10">
         <v>4</v>
       </c>
-      <c r="G70" s="31">
+      <c r="G70" s="29">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H70" s="30">
+      <c r="H70" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -2992,7 +2999,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="19">
+      <c r="A71" s="18">
         <v>69</v>
       </c>
       <c r="B71" s="9">
@@ -3010,11 +3017,11 @@
       <c r="F71" s="10">
         <v>4</v>
       </c>
-      <c r="G71" s="31">
+      <c r="G71" s="29">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H71" s="30">
+      <c r="H71" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -3024,7 +3031,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="19">
+      <c r="A72" s="18">
         <v>70</v>
       </c>
       <c r="B72" s="9">
@@ -3042,11 +3049,11 @@
       <c r="F72" s="10">
         <v>7</v>
       </c>
-      <c r="G72" s="31">
+      <c r="G72" s="29">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="H72" s="30">
+      <c r="H72" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3056,7 +3063,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="19">
+      <c r="A73" s="18">
         <v>71</v>
       </c>
       <c r="B73" s="9">
@@ -3074,11 +3081,11 @@
       <c r="F73" s="10">
         <v>4</v>
       </c>
-      <c r="G73" s="31">
+      <c r="G73" s="29">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H73" s="30">
+      <c r="H73" s="29">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -3088,7 +3095,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="19">
+      <c r="A74" s="18">
         <v>72</v>
       </c>
       <c r="B74" s="9">
@@ -3106,11 +3113,11 @@
       <c r="F74" s="10">
         <v>6</v>
       </c>
-      <c r="G74" s="31">
+      <c r="G74" s="29">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H74" s="30">
+      <c r="H74" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3120,7 +3127,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="19">
+      <c r="A75" s="18">
         <v>73</v>
       </c>
       <c r="B75" s="9">
@@ -3138,11 +3145,11 @@
       <c r="F75" s="10">
         <v>3</v>
       </c>
-      <c r="G75" s="31">
+      <c r="G75" s="29">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="H75" s="30">
+      <c r="H75" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -3152,7 +3159,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="19">
+      <c r="A76" s="18">
         <v>74</v>
       </c>
       <c r="B76" s="9">
@@ -3170,11 +3177,11 @@
       <c r="F76" s="10">
         <v>5</v>
       </c>
-      <c r="G76" s="31">
+      <c r="G76" s="29">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="H76" s="30">
+      <c r="H76" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3184,7 +3191,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="19">
+      <c r="A77" s="18">
         <v>75</v>
       </c>
       <c r="B77" s="9">
@@ -3202,11 +3209,11 @@
       <c r="F77" s="10">
         <v>4</v>
       </c>
-      <c r="G77" s="31">
+      <c r="G77" s="29">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H77" s="30">
+      <c r="H77" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3216,7 +3223,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="19">
+      <c r="A78" s="18">
         <v>76</v>
       </c>
       <c r="B78" s="9">
@@ -3234,11 +3241,11 @@
       <c r="F78" s="10">
         <v>1</v>
       </c>
-      <c r="G78" s="31">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="H78" s="30">
+      <c r="G78" s="29">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H78" s="29">
         <v>1</v>
       </c>
       <c r="I78" s="3"/>
@@ -3247,7 +3254,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="19">
+      <c r="A79" s="18">
         <v>77</v>
       </c>
       <c r="B79" s="9">
@@ -3265,11 +3272,11 @@
       <c r="F79" s="10">
         <v>1</v>
       </c>
-      <c r="G79" s="31">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="H79" s="30">
+      <c r="G79" s="29">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H79" s="29">
         <v>1</v>
       </c>
       <c r="I79" s="3"/>
@@ -3278,7 +3285,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="19">
+      <c r="A80" s="18">
         <v>78</v>
       </c>
       <c r="B80" s="9">
@@ -3296,11 +3303,11 @@
       <c r="F80" s="10">
         <v>5</v>
       </c>
-      <c r="G80" s="31">
+      <c r="G80" s="29">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H80" s="30">
+      <c r="H80" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3310,7 +3317,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="19">
+      <c r="A81" s="18">
         <v>79</v>
       </c>
       <c r="B81" s="9">
@@ -3328,11 +3335,11 @@
       <c r="F81" s="10">
         <v>5</v>
       </c>
-      <c r="G81" s="31">
+      <c r="G81" s="29">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="H81" s="30">
+      <c r="H81" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3342,7 +3349,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="19">
+      <c r="A82" s="18">
         <v>80</v>
       </c>
       <c r="B82" s="9">
@@ -3360,11 +3367,11 @@
       <c r="F82" s="10">
         <v>6</v>
       </c>
-      <c r="G82" s="31">
+      <c r="G82" s="29">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H82" s="30">
+      <c r="H82" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3374,7 +3381,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="19">
+      <c r="A83" s="18">
         <v>81</v>
       </c>
       <c r="B83" s="9">
@@ -3392,11 +3399,11 @@
       <c r="F83" s="10">
         <v>6</v>
       </c>
-      <c r="G83" s="31">
+      <c r="G83" s="29">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H83" s="30">
+      <c r="H83" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3406,7 +3413,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="19">
+      <c r="A84" s="18">
         <v>82</v>
       </c>
       <c r="B84" s="9">
@@ -3424,11 +3431,11 @@
       <c r="F84" s="10">
         <v>3</v>
       </c>
-      <c r="G84" s="31">
+      <c r="G84" s="29">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H84" s="30">
+      <c r="H84" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3438,7 +3445,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="19">
+      <c r="A85" s="18">
         <v>83</v>
       </c>
       <c r="B85" s="9">
@@ -3456,11 +3463,11 @@
       <c r="F85" s="10">
         <v>6</v>
       </c>
-      <c r="G85" s="31">
+      <c r="G85" s="29">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H85" s="30">
+      <c r="H85" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3470,7 +3477,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="19">
+      <c r="A86" s="18">
         <v>84</v>
       </c>
       <c r="B86" s="9">
@@ -3488,11 +3495,11 @@
       <c r="F86" s="10">
         <v>3</v>
       </c>
-      <c r="G86" s="31">
+      <c r="G86" s="29">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H86" s="30">
+      <c r="H86" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3502,7 +3509,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="19">
+      <c r="A87" s="18">
         <v>85</v>
       </c>
       <c r="B87" s="9">
@@ -3520,11 +3527,11 @@
       <c r="F87" s="10">
         <v>2</v>
       </c>
-      <c r="G87" s="31">
+      <c r="G87" s="29">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="H87" s="30">
+      <c r="H87" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -3534,7 +3541,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="19">
+      <c r="A88" s="18">
         <v>86</v>
       </c>
       <c r="B88" s="9">
@@ -3552,11 +3559,11 @@
       <c r="F88" s="10">
         <v>4</v>
       </c>
-      <c r="G88" s="31">
+      <c r="G88" s="29">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="H88" s="30">
+      <c r="H88" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3566,7 +3573,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="19">
+      <c r="A89" s="18">
         <v>87</v>
       </c>
       <c r="B89" s="9">
@@ -3584,11 +3591,11 @@
       <c r="F89" s="10">
         <v>3</v>
       </c>
-      <c r="G89" s="31">
+      <c r="G89" s="29">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="H89" s="30">
+      <c r="H89" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3598,7 +3605,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="19">
+      <c r="A90" s="18">
         <v>88</v>
       </c>
       <c r="B90" s="9">
@@ -3616,11 +3623,11 @@
       <c r="F90" s="10">
         <v>2</v>
       </c>
-      <c r="G90" s="31">
+      <c r="G90" s="29">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="H90" s="30">
+      <c r="H90" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3630,7 +3637,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="19">
+      <c r="A91" s="18">
         <v>89</v>
       </c>
       <c r="B91" s="9">
@@ -3648,11 +3655,11 @@
       <c r="F91" s="10">
         <v>4</v>
       </c>
-      <c r="G91" s="31">
+      <c r="G91" s="29">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H91" s="30">
+      <c r="H91" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3662,7 +3669,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="19">
+      <c r="A92" s="18">
         <v>90</v>
       </c>
       <c r="B92" s="9">
@@ -3680,11 +3687,11 @@
       <c r="F92" s="10">
         <v>2</v>
       </c>
-      <c r="G92" s="31">
+      <c r="G92" s="29">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="H92" s="30">
+      <c r="H92" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3694,7 +3701,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="19">
+      <c r="A93" s="18">
         <v>91</v>
       </c>
       <c r="B93" s="9">
@@ -3712,11 +3719,11 @@
       <c r="F93" s="10">
         <v>5</v>
       </c>
-      <c r="G93" s="31">
+      <c r="G93" s="29">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="H93" s="30">
+      <c r="H93" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3726,7 +3733,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="19">
+      <c r="A94" s="18">
         <v>92</v>
       </c>
       <c r="B94" s="9">
@@ -3744,11 +3751,11 @@
       <c r="F94" s="10">
         <v>5</v>
       </c>
-      <c r="G94" s="31">
+      <c r="G94" s="29">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H94" s="30">
+      <c r="H94" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3758,7 +3765,7 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="19">
+      <c r="A95" s="18">
         <v>93</v>
       </c>
       <c r="B95" s="9">
@@ -3776,11 +3783,11 @@
       <c r="F95" s="10">
         <v>4</v>
       </c>
-      <c r="G95" s="31">
+      <c r="G95" s="29">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="H95" s="30">
+      <c r="H95" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -3789,8 +3796,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="19">
+    <row r="96" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="18">
         <v>94</v>
       </c>
       <c r="B96" s="9">
@@ -3808,11 +3815,11 @@
       <c r="F96" s="10">
         <v>4</v>
       </c>
-      <c r="G96" s="31">
+      <c r="G96" s="29">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="H96" s="30">
+      <c r="H96" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3822,7 +3829,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="19">
+      <c r="A97" s="18">
         <v>95</v>
       </c>
       <c r="B97" s="9">
@@ -3840,11 +3847,11 @@
       <c r="F97" s="10">
         <v>4</v>
       </c>
-      <c r="G97" s="31">
+      <c r="G97" s="29">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="H97" s="30">
+      <c r="H97" s="29">
         <v>1</v>
       </c>
       <c r="I97" s="3"/>
@@ -3853,7 +3860,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="19">
+      <c r="A98" s="18">
         <v>96</v>
       </c>
       <c r="B98" s="9">
@@ -3871,11 +3878,11 @@
       <c r="F98" s="10">
         <v>4</v>
       </c>
-      <c r="G98" s="31">
+      <c r="G98" s="30">
         <f t="shared" si="2"/>
         <v>24.5</v>
       </c>
-      <c r="H98" s="31">
+      <c r="H98" s="30">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3885,7 +3892,7 @@
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="19">
+      <c r="A99" s="18">
         <v>97</v>
       </c>
       <c r="B99" s="9">
@@ -3903,11 +3910,11 @@
       <c r="F99" s="10">
         <v>6</v>
       </c>
-      <c r="G99" s="31">
+      <c r="G99" s="29">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H99" s="30">
+      <c r="H99" s="29">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -3917,7 +3924,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="19">
+      <c r="A100" s="18">
         <v>98</v>
       </c>
       <c r="B100" s="9">
@@ -3935,11 +3942,11 @@
       <c r="F100" s="10">
         <v>4</v>
       </c>
-      <c r="G100" s="31">
+      <c r="G100" s="29">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="H100" s="30">
+      <c r="H100" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3949,7 +3956,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="19">
+      <c r="A101" s="18">
         <v>99</v>
       </c>
       <c r="B101" s="9">
@@ -3967,11 +3974,11 @@
       <c r="F101" s="10">
         <v>7</v>
       </c>
-      <c r="G101" s="31">
+      <c r="G101" s="29">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="H101" s="30">
+      <c r="H101" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -3981,7 +3988,7 @@
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="19">
+      <c r="A102" s="18">
         <v>100</v>
       </c>
       <c r="B102" s="9">
@@ -3999,11 +4006,11 @@
       <c r="F102" s="10">
         <v>6</v>
       </c>
-      <c r="G102" s="31">
+      <c r="G102" s="29">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H102" s="30">
+      <c r="H102" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4013,7 +4020,7 @@
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="19">
+      <c r="A103" s="18">
         <v>101</v>
       </c>
       <c r="B103" s="9">
@@ -4031,11 +4038,11 @@
       <c r="F103" s="10">
         <v>6</v>
       </c>
-      <c r="G103" s="31">
+      <c r="G103" s="29">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H103" s="30">
+      <c r="H103" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4045,7 +4052,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="19">
+      <c r="A104" s="18">
         <v>102</v>
       </c>
       <c r="B104" s="9">
@@ -4063,11 +4070,11 @@
       <c r="F104" s="10">
         <v>6</v>
       </c>
-      <c r="G104" s="31">
+      <c r="G104" s="29">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="H104" s="30">
+      <c r="H104" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -4077,7 +4084,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="19">
+      <c r="A105" s="18">
         <v>103</v>
       </c>
       <c r="B105" s="9">
@@ -4095,11 +4102,11 @@
       <c r="F105" s="10">
         <v>3</v>
       </c>
-      <c r="G105" s="31">
+      <c r="G105" s="29">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="H105" s="30">
+      <c r="H105" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4109,7 +4116,7 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="19">
+      <c r="A106" s="18">
         <v>104</v>
       </c>
       <c r="B106" s="9">
@@ -4127,11 +4134,11 @@
       <c r="F106" s="10">
         <v>5</v>
       </c>
-      <c r="G106" s="31">
+      <c r="G106" s="30">
         <f t="shared" si="2"/>
         <v>27.5</v>
       </c>
-      <c r="H106" s="31">
+      <c r="H106" s="30">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -4141,7 +4148,7 @@
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="19">
+      <c r="A107" s="18">
         <v>105</v>
       </c>
       <c r="B107" s="9">
@@ -4159,11 +4166,11 @@
       <c r="F107" s="10">
         <v>4</v>
       </c>
-      <c r="G107" s="31">
+      <c r="G107" s="30">
         <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
-      <c r="H107" s="31">
+      <c r="H107" s="30">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
@@ -4173,7 +4180,7 @@
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="19">
+      <c r="A108" s="18">
         <v>106</v>
       </c>
       <c r="B108" s="9">
@@ -4191,11 +4198,11 @@
       <c r="F108" s="10">
         <v>6</v>
       </c>
-      <c r="G108" s="31">
+      <c r="G108" s="29">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H108" s="30">
+      <c r="H108" s="29">
         <v>1</v>
       </c>
       <c r="I108" s="3"/>
@@ -4204,7 +4211,7 @@
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="19">
+      <c r="A109" s="18">
         <v>107</v>
       </c>
       <c r="B109" s="9">
@@ -4222,11 +4229,11 @@
       <c r="F109" s="10">
         <v>6</v>
       </c>
-      <c r="G109" s="31">
+      <c r="G109" s="29">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="H109" s="30">
+      <c r="H109" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4236,7 +4243,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="19">
+      <c r="A110" s="18">
         <v>108</v>
       </c>
       <c r="B110" s="9">
@@ -4254,11 +4261,11 @@
       <c r="F110" s="10">
         <v>7</v>
       </c>
-      <c r="G110" s="31">
+      <c r="G110" s="29">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="H110" s="30">
+      <c r="H110" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4268,7 +4275,7 @@
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="19">
+      <c r="A111" s="18">
         <v>109</v>
       </c>
       <c r="B111" s="9">
@@ -4286,11 +4293,11 @@
       <c r="F111" s="10">
         <v>7</v>
       </c>
-      <c r="G111" s="31">
+      <c r="G111" s="29">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="H111" s="30">
+      <c r="H111" s="29">
         <v>1</v>
       </c>
       <c r="I111" s="3"/>
@@ -4299,7 +4306,7 @@
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="19">
+      <c r="A112" s="18">
         <v>110</v>
       </c>
       <c r="B112" s="9">
@@ -4317,11 +4324,11 @@
       <c r="F112" s="10">
         <v>6</v>
       </c>
-      <c r="G112" s="31">
+      <c r="G112" s="29">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H112" s="30">
+      <c r="H112" s="29">
         <v>1</v>
       </c>
       <c r="I112" s="3"/>
@@ -4330,7 +4337,7 @@
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="19">
+      <c r="A113" s="18">
         <v>111</v>
       </c>
       <c r="B113" s="9">
@@ -4348,11 +4355,11 @@
       <c r="F113" s="10">
         <v>6</v>
       </c>
-      <c r="G113" s="31">
+      <c r="G113" s="29">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H113" s="30">
+      <c r="H113" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -4362,7 +4369,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="19">
+      <c r="A114" s="18">
         <v>112</v>
       </c>
       <c r="B114" s="9">
@@ -4380,11 +4387,11 @@
       <c r="F114" s="10">
         <v>5</v>
       </c>
-      <c r="G114" s="31">
+      <c r="G114" s="29">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H114" s="30">
+      <c r="H114" s="29">
         <v>1</v>
       </c>
       <c r="I114" s="3"/>
@@ -4393,7 +4400,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="19">
+      <c r="A115" s="18">
         <v>113</v>
       </c>
       <c r="B115" s="9">
@@ -4411,11 +4418,11 @@
       <c r="F115" s="10">
         <v>4</v>
       </c>
-      <c r="G115" s="31">
+      <c r="G115" s="29">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H115" s="30">
+      <c r="H115" s="29">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -4425,7 +4432,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="19">
+      <c r="A116" s="18">
         <v>114</v>
       </c>
       <c r="B116" s="9">
@@ -4443,11 +4450,11 @@
       <c r="F116" s="10">
         <v>5</v>
       </c>
-      <c r="G116" s="31">
+      <c r="G116" s="29">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H116" s="30">
+      <c r="H116" s="29">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -4457,7 +4464,7 @@
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="19">
+      <c r="A117" s="18">
         <v>115</v>
       </c>
       <c r="B117" s="9">
@@ -4475,11 +4482,11 @@
       <c r="F117" s="10">
         <v>4</v>
       </c>
-      <c r="G117" s="31">
+      <c r="G117" s="29">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H117" s="30">
+      <c r="H117" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -4489,7 +4496,7 @@
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="19">
+      <c r="A118" s="18">
         <v>116</v>
       </c>
       <c r="B118" s="9">
@@ -4507,11 +4514,11 @@
       <c r="F118" s="10">
         <v>1</v>
       </c>
-      <c r="G118" s="31">
+      <c r="G118" s="29">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="H118" s="30">
+      <c r="H118" s="29">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
@@ -4521,7 +4528,7 @@
       </c>
     </row>
     <row r="119" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="22">
+      <c r="A119" s="21">
         <v>117</v>
       </c>
       <c r="B119" s="11">
@@ -4539,11 +4546,11 @@
       <c r="F119" s="13">
         <v>5</v>
       </c>
-      <c r="G119" s="31">
+      <c r="G119" s="29">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H119" s="30">
+      <c r="H119" s="29">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -4553,64 +4560,70 @@
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="23" t="s">
+      <c r="A120" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B120" s="25">
+      <c r="B120" s="24">
         <f>SUM(B3:B119)</f>
         <v>543.5</v>
       </c>
-      <c r="C120" s="25">
+      <c r="C120" s="24">
         <f t="shared" ref="C120:G120" si="4">SUM(C3:C119)</f>
         <v>591</v>
       </c>
-      <c r="D120" s="25">
+      <c r="D120" s="24">
         <f t="shared" si="4"/>
         <v>564</v>
       </c>
-      <c r="E120" s="25">
+      <c r="E120" s="24">
         <f t="shared" si="4"/>
         <v>497.5</v>
       </c>
-      <c r="F120" s="25">
+      <c r="F120" s="24">
         <f t="shared" si="4"/>
         <v>534</v>
       </c>
-      <c r="G120" s="27">
+      <c r="G120" s="26">
         <f t="shared" si="4"/>
         <v>2730</v>
       </c>
-      <c r="H120" s="29"/>
+      <c r="H120" s="29">
+        <f>SQRT(G120)</f>
+        <v>52.249401910452526</v>
+      </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="24" t="s">
+      <c r="A121" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B121" s="26">
+      <c r="B121" s="25">
         <f>_xlfn.VAR.P(B3:B119)</f>
         <v>2.0600847395719191</v>
       </c>
-      <c r="C121" s="26">
+      <c r="C121" s="25">
         <f t="shared" ref="C121:F121" si="5">_xlfn.VAR.P(C3:C119)</f>
         <v>2.23241288625904</v>
       </c>
-      <c r="D121" s="26">
+      <c r="D121" s="25">
         <f t="shared" si="5"/>
         <v>2.5575279421433268</v>
       </c>
-      <c r="E121" s="26">
+      <c r="E121" s="25">
         <f t="shared" si="5"/>
         <v>2.793264665059537</v>
       </c>
-      <c r="F121" s="26">
+      <c r="F121" s="25">
         <f t="shared" si="5"/>
         <v>2.9638395792241945</v>
       </c>
-      <c r="G121" s="28">
+      <c r="G121" s="27">
         <f>SUM(B121:F121)</f>
         <v>12.607129812258018</v>
       </c>
-      <c r="H121" s="29"/>
+      <c r="H121" s="30">
+        <f>(MAX(B121:F121)-MIN(B121:F121))/2</f>
+        <v>0.45187741982613772</v>
+      </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="17" t="s">
@@ -4636,7 +4649,7 @@
         <f t="shared" si="6"/>
         <v>4.5641025641025639</v>
       </c>
-      <c r="H122" s="29"/>
+      <c r="H122" s="28"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
@@ -4662,7 +4675,7 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="H123" s="29"/>
+      <c r="H123" s="28"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
@@ -4688,7 +4701,7 @@
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="H124" s="29"/>
+      <c r="H124" s="28"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
@@ -4714,33 +4727,33 @@
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="H125" s="29"/>
+      <c r="H125" s="28"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="17" t="s">
+      <c r="A126" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B126" s="14">
+      <c r="B126" s="33">
         <f>B125/2</f>
         <v>3</v>
       </c>
-      <c r="C126" s="14">
+      <c r="C126" s="33">
         <f t="shared" ref="C126:F126" si="10">C125/2</f>
         <v>3</v>
       </c>
-      <c r="D126" s="14">
+      <c r="D126" s="33">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="E126" s="14">
+      <c r="E126" s="33">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="F126" s="14">
+      <c r="F126" s="33">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="H126" s="29"/>
+      <c r="H126" s="28"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">

</xml_diff>